<commit_message>
further work on led layout
</commit_message>
<xml_diff>
--- a/LEDs.xlsx
+++ b/LEDs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="600" windowWidth="28215" windowHeight="13740" activeTab="2"/>
+    <workbookView xWindow="270" yWindow="600" windowWidth="28215" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Kenndaten" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="123">
   <si>
     <t>Quelle</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Gesamtanteil</t>
   </si>
   <si>
-    <t>Pattern</t>
-  </si>
-  <si>
     <t>gesamt</t>
   </si>
   <si>
@@ -337,9 +334,6 @@
     <t>618nm</t>
   </si>
   <si>
-    <t>LED SMD 3529</t>
-  </si>
-  <si>
     <t>LED SMD 0,5 11BL</t>
   </si>
   <si>
@@ -349,9 +343,6 @@
     <t>LED SMD 3535</t>
   </si>
   <si>
-    <t>LED SMD 3536</t>
-  </si>
-  <si>
     <t>LED SMD 1W 60RT</t>
   </si>
   <si>
@@ -368,6 +359,33 @@
   </si>
   <si>
     <t>PLCC-6 (5050)</t>
+  </si>
+  <si>
+    <t>Leistung (W)</t>
+  </si>
+  <si>
+    <t>Lichtstrom (lm)</t>
+  </si>
+  <si>
+    <t>EinzelLEDs Everstar 5730 0.5W</t>
+  </si>
+  <si>
+    <t>IKEA VÄXER 10W</t>
+  </si>
+  <si>
+    <t>Weissanteil</t>
+  </si>
+  <si>
+    <t>IKEA VÄXER 16W</t>
+  </si>
+  <si>
+    <t>lumen</t>
+  </si>
+  <si>
+    <t>lumen gesamt</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
   </si>
 </sst>
 </file>
@@ -495,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -536,6 +554,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -555,7 +582,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -591,15 +618,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
@@ -607,15 +625,30 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20 % - Akzent5" xfId="3" builtinId="46"/>
@@ -646,15 +679,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -676,7 +709,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="85725" y="3590925"/>
+          <a:off x="419100" y="3752850"/>
           <a:ext cx="3333750" cy="2000250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -986,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -999,9 +1032,12 @@
     <col min="3" max="3" width="7.75" customWidth="1"/>
     <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.75" customWidth="1"/>
+    <col min="7" max="7" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1009,7 +1045,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1017,7 +1053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1026,12 +1062,17 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75">
+    <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="F10" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="25" t="s">
         <v>4</v>
       </c>
@@ -1047,11 +1088,23 @@
       <c r="E11" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1062,22 +1115,33 @@
         <v>140</v>
       </c>
       <c r="D12" s="23">
-        <f>C12/$C$17</f>
+        <f>C12/$C$19</f>
         <v>0.27777777777777779</v>
       </c>
       <c r="E12" s="23">
         <f>C12/SUM($C$12:$C$14)</f>
         <v>0.35714285714285715</v>
       </c>
-      <c r="F12">
-        <v>18</v>
-      </c>
-      <c r="G12" s="23">
-        <f>F12/$F$17</f>
-        <v>0.2857142857142857</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12" s="50">
+        <v>12</v>
+      </c>
+      <c r="G12" s="34">
+        <v>55</v>
+      </c>
+      <c r="H12" s="34">
+        <f>F12*G12</f>
+        <v>660</v>
+      </c>
+      <c r="I12" s="23">
+        <f>F12/$F$20</f>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="J12" s="23">
+        <f>F12/SUM(F$12:F$14)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1088,22 +1152,33 @@
         <v>204</v>
       </c>
       <c r="D13" s="23">
-        <f>C13/$C$17</f>
+        <f>C13/$C$19</f>
         <v>0.40476190476190477</v>
       </c>
       <c r="E13" s="23">
         <f t="shared" ref="E13:E14" si="0">C13/SUM($C$12:$C$14)</f>
         <v>0.52040816326530615</v>
       </c>
-      <c r="F13">
-        <v>25</v>
-      </c>
-      <c r="G13" s="23">
-        <f t="shared" ref="G13:G16" si="1">F13/$F$17</f>
-        <v>0.3968253968253968</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="F13" s="50">
+        <v>18</v>
+      </c>
+      <c r="G13" s="34">
+        <v>55</v>
+      </c>
+      <c r="H13" s="34">
+        <f t="shared" ref="H13:H18" si="1">F13*G13</f>
+        <v>990</v>
+      </c>
+      <c r="I13" s="23">
+        <f t="shared" ref="I13:I14" si="2">F13/$F$20</f>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="J13" s="23">
+        <f t="shared" ref="J13:J14" si="3">F13/SUM(F$12:F$14)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1114,83 +1189,178 @@
         <v>48</v>
       </c>
       <c r="D14" s="23">
-        <f>C14/$C$17</f>
+        <f>C14/$C$19</f>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="E14" s="23">
         <f t="shared" si="0"/>
         <v>0.12244897959183673</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="50">
         <v>6</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="34">
+        <v>55</v>
+      </c>
+      <c r="H14" s="34">
         <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="I14" s="23">
+        <f t="shared" si="2"/>
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="J14" s="23">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="50">
+        <f>SUM(F12:F14)</f>
+        <v>36</v>
+      </c>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17">
+        <v>48</v>
+      </c>
+      <c r="D17" s="23">
+        <f>C17/$C$19</f>
         <v>9.5238095238095233E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15">
-        <v>48</v>
-      </c>
-      <c r="D15" s="23">
-        <f>C15/$C$17</f>
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>92</v>
       </c>
-      <c r="F15">
+      <c r="F17" s="50">
+        <v>4</v>
+      </c>
+      <c r="G17" s="40">
+        <v>4</v>
+      </c>
+      <c r="H17" s="34">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I17" s="23">
+        <f>F17/$F$20</f>
+        <v>8.6956521739130432E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18">
+        <v>64</v>
+      </c>
+      <c r="D18" s="23">
+        <f>C18/$C$19</f>
+        <v>0.12698412698412698</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="50">
         <v>6</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G18" s="40">
+        <v>11</v>
+      </c>
+      <c r="H18" s="34">
         <f t="shared" si="1"/>
-        <v>9.5238095238095233E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16">
-        <v>64</v>
-      </c>
-      <c r="D16" s="23">
-        <f>C16/$C$17</f>
-        <v>0.12698412698412698</v>
-      </c>
-      <c r="E16" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16">
-        <v>8</v>
-      </c>
-      <c r="G16" s="23">
-        <f t="shared" si="1"/>
-        <v>0.12698412698412698</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="15">
-      <c r="B17" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="23">
+        <f>F18/$F$20</f>
+        <v>0.13043478260869565</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15">
+      <c r="B19" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="21">
-        <f>SUM(C12:C16)</f>
+      <c r="C19" s="21">
+        <f>SUM(C12:C18)</f>
         <v>504</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="F17">
-        <f>SUM(F12:F16)</f>
-        <v>63</v>
+      <c r="D19" s="24"/>
+      <c r="F19" s="54">
+        <f>SUM(F17:F18)</f>
+        <v>10</v>
+      </c>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+    </row>
+    <row r="20" spans="1:9" ht="15">
+      <c r="B20" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="24"/>
+      <c r="F20" s="55">
+        <f>F19+F15</f>
+        <v>46</v>
+      </c>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+    </row>
+    <row r="21" spans="1:9" ht="15">
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21">
+        <v>35</v>
+      </c>
+      <c r="F21" s="21">
+        <f>0.5*F19</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15">
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22">
+        <v>2580</v>
+      </c>
+      <c r="H22" s="21">
+        <f>SUM(H12:H18)</f>
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1695,7 +1865,7 @@
       </c>
       <c r="D16" s="10"/>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="1" t="s">
@@ -1729,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1801,10 +1971,10 @@
         <v>9</v>
       </c>
       <c r="O2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" t="s">
         <v>95</v>
-      </c>
-      <c r="P2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15">
@@ -1847,7 +2017,7 @@
       <c r="N3" s="2">
         <v>0.1</v>
       </c>
-      <c r="O3" s="34">
+      <c r="O3" s="46">
         <f>Kenndaten!$B$4/'SMD LEDs'!J3</f>
         <v>90.909090909090907</v>
       </c>
@@ -1896,7 +2066,7 @@
       <c r="N4" s="2">
         <v>0.1</v>
       </c>
-      <c r="O4" s="34"/>
+      <c r="O4" s="46"/>
       <c r="P4" s="19">
         <f>ROUNDUP(Kenndaten!E13*'SMD LEDs'!$O$3,0)</f>
         <v>48</v>
@@ -1941,7 +2111,7 @@
       <c r="N5" s="31">
         <v>0.1</v>
       </c>
-      <c r="O5" s="35"/>
+      <c r="O5" s="47"/>
       <c r="P5" s="19">
         <f>ROUNDUP(Kenndaten!E14*'SMD LEDs'!$O$3,0)</f>
         <v>12</v>
@@ -1957,42 +2127,42 @@
       <c r="C6">
         <v>121341</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="36">
         <v>17500</v>
       </c>
-      <c r="I6" s="37">
+      <c r="I6" s="34">
         <v>120</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="37">
         <v>55</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="34">
         <v>3</v>
       </c>
-      <c r="L6" s="37">
+      <c r="L6" s="34">
         <v>150</v>
       </c>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41">
+      <c r="M6" s="38"/>
+      <c r="N6" s="38">
         <v>0.18</v>
       </c>
-      <c r="O6" s="33">
+      <c r="O6" s="48">
         <f>Kenndaten!$B$4/'SMD LEDs'!J6</f>
         <v>36.363636363636367</v>
       </c>
-      <c r="P6" s="42">
+      <c r="P6" s="39">
         <f>ROUNDUP(Kenndaten!E12*'SMD LEDs'!$O$6,0)</f>
         <v>13</v>
       </c>
@@ -2007,37 +2177,37 @@
       <c r="C7">
         <v>121340</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="36">
         <v>17500</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="34">
         <v>120</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="37">
         <v>55</v>
       </c>
-      <c r="K7" s="44">
+      <c r="K7" s="40">
         <v>3</v>
       </c>
-      <c r="L7" s="37">
+      <c r="L7" s="34">
         <v>150</v>
       </c>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41">
+      <c r="M7" s="38"/>
+      <c r="N7" s="38">
         <v>0.18</v>
       </c>
-      <c r="O7" s="43"/>
-      <c r="P7" s="42">
+      <c r="O7" s="49"/>
+      <c r="P7" s="39">
         <f>ROUNDUP(Kenndaten!E13*'SMD LEDs'!$O$6,0)</f>
         <v>19</v>
       </c>
@@ -2061,7 +2231,7 @@
       <c r="G8" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="36">
         <v>17500</v>
       </c>
       <c r="I8" s="26">
@@ -2080,7 +2250,7 @@
       <c r="N8" s="31">
         <v>0.18</v>
       </c>
-      <c r="O8" s="35"/>
+      <c r="O8" s="47"/>
       <c r="P8" s="32">
         <f>ROUNDUP(Kenndaten!E14*'SMD LEDs'!$O$6,0)</f>
         <v>5</v>
@@ -2088,19 +2258,19 @@
     </row>
     <row r="9" spans="1:16" ht="15">
       <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
         <v>97</v>
       </c>
-      <c r="B9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>116</v>
+      <c r="E9" s="40" t="s">
+        <v>113</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>3500</v>
@@ -2115,7 +2285,7 @@
         <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M9" s="2">
         <v>0.2</v>
@@ -2123,13 +2293,13 @@
     </row>
     <row r="10" spans="1:16" ht="15">
       <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="B10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>116</v>
+      <c r="E10" s="40" t="s">
+        <v>113</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>25</v>
@@ -2150,7 +2320,7 @@
         <v>3.3</v>
       </c>
       <c r="L10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M10" s="2">
         <v>0.2</v>
@@ -2158,19 +2328,19 @@
     </row>
     <row r="11" spans="1:16" ht="15">
       <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
         <v>97</v>
       </c>
-      <c r="B11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>115</v>
+      <c r="E11" s="40" t="s">
+        <v>112</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H11" s="1">
         <v>600</v>
@@ -2184,17 +2354,17 @@
     </row>
     <row r="12" spans="1:16" ht="15">
       <c r="A12" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>97</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>98</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="47" t="s">
+      <c r="E12" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="43" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="29" t="s">
@@ -2221,19 +2391,19 @@
         <v>38</v>
       </c>
       <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
         <v>102</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="F13" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F13" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="H13" s="1">
         <v>3500</v>
@@ -2259,19 +2429,19 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>103</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H14" s="1">
         <v>1400</v>
@@ -2300,12 +2470,12 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="41" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -2338,13 +2508,13 @@
         <v>43</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D16" s="26"/>
-      <c r="E16" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="47" t="s">
+      <c r="E16" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="43" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="29" t="s">
@@ -2373,16 +2543,16 @@
       <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:14" ht="15">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="45" t="s">
+      <c r="F17" s="41" t="s">
         <v>28</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -2391,33 +2561,33 @@
       <c r="H17" s="1">
         <v>6000</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="40">
         <v>120</v>
       </c>
       <c r="J17" s="20">
         <v>19</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="40">
         <v>2.2000000000000002</v>
       </c>
       <c r="L17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N17" s="2">
         <v>0.27</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="45" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -2426,7 +2596,7 @@
       <c r="H18" s="1">
         <v>7000</v>
       </c>
-      <c r="I18" s="44">
+      <c r="I18" s="40">
         <v>120</v>
       </c>
       <c r="J18" s="20">
@@ -2436,23 +2606,23 @@
         <v>3.2</v>
       </c>
       <c r="L18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N18" s="2">
         <v>0.33</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15">
-      <c r="A19" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="45" t="s">
+      <c r="A19" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="41" t="s">
         <v>28</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -2461,33 +2631,33 @@
       <c r="H19" s="1">
         <v>1500</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="40">
         <v>120</v>
       </c>
       <c r="J19" s="20">
         <v>4.7</v>
       </c>
-      <c r="K19" s="44">
+      <c r="K19" s="40">
         <v>2.2000000000000002</v>
       </c>
       <c r="L19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N19" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15">
-      <c r="A20" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="49" t="s">
+      <c r="A20" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="45" t="s">
         <v>25</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -2496,7 +2666,7 @@
       <c r="H20" s="1">
         <v>1000</v>
       </c>
-      <c r="I20" s="44">
+      <c r="I20" s="40">
         <v>120</v>
       </c>
       <c r="J20" s="20">
@@ -2506,7 +2676,7 @@
         <v>3.2</v>
       </c>
       <c r="L20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N20" s="2">
         <v>0.33</v>

</xml_diff>